<commit_message>
EPBDS-7880 Create the test case check the order in collect result smart rules
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7801_Collect_in_Simple_and_Smart_Lookups.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7801_Collect_in_Simple_and_Smart_Lookups.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpikus\.openl-webstudio\user-workspace\admin\EPBDS-7801\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="27795" windowHeight="12075"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="27795" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="74">
   <si>
     <t>Plan</t>
   </si>
@@ -231,12 +226,24 @@
   </si>
   <si>
     <t>500, 500, 500, 500</t>
+  </si>
+  <si>
+    <t>Test CarPrice checkOrder</t>
+  </si>
+  <si>
+    <t>_res_[0]</t>
+  </si>
+  <si>
+    <t>_res_[1]</t>
+  </si>
+  <si>
+    <t>_res_[2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
@@ -474,6 +481,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="9" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="6" fontId="1" fillId="9" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -482,12 +511,6 @@
     </xf>
     <xf numFmtId="6" fontId="1" fillId="9" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -510,25 +533,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="9" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 5" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
@@ -573,9 +580,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -613,9 +620,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -650,7 +657,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -685,7 +692,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -859,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:G83"/>
+  <dimension ref="B5:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,85 +881,85 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="20" t="s">
         <v>12</v>
       </c>
     </row>
@@ -967,38 +974,38 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="15" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1008,7 +1015,7 @@
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="26"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
@@ -1018,7 +1025,7 @@
       <c r="D22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="13" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1030,7 +1037,7 @@
       <c r="D23" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1042,7 +1049,7 @@
       <c r="D24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1054,7 +1061,7 @@
       <c r="D25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1066,7 +1073,7 @@
       <c r="D26" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="13" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1078,39 +1085,39 @@
       <c r="D27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="18" t="s">
+      <c r="E31" s="33"/>
+      <c r="F31" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="20"/>
+      <c r="G31" s="34"/>
     </row>
     <row r="32" spans="2:7" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="15"/>
-      <c r="C32" s="17"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="31"/>
       <c r="D32" s="1" t="s">
         <v>32</v>
       </c>
@@ -1137,10 +1144,10 @@
       <c r="E33" s="4">
         <v>45750</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="25">
         <v>93200</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="25">
         <v>90400</v>
       </c>
     </row>
@@ -1157,8 +1164,8 @@
       <c r="E34" s="4">
         <v>44050</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
@@ -1173,8 +1180,8 @@
       <c r="E35" s="4">
         <v>46550</v>
       </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1237,52 +1244,52 @@
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="D42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="27" t="s">
+      <c r="E42" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F42" s="27" t="s">
+      <c r="F42" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G42" s="27" t="s">
+      <c r="G42" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="28" t="s">
+      <c r="F43" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G43" s="28" t="s">
+      <c r="G43" s="15" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1290,17 +1297,17 @@
       <c r="B44" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="16" t="s">
         <v>56</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="26"/>
+      <c r="G44" s="13"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D45" s="7" t="s">
@@ -1312,7 +1319,7 @@
       <c r="F45" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G45" s="26">
+      <c r="G45" s="13">
         <v>51650</v>
       </c>
     </row>
@@ -1330,7 +1337,7 @@
       <c r="F46" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G46" s="26">
+      <c r="G46" s="13">
         <v>93200</v>
       </c>
     </row>
@@ -1348,7 +1355,7 @@
       <c r="F47" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G47" s="26">
+      <c r="G47" s="13">
         <v>93200</v>
       </c>
     </row>
@@ -1366,7 +1373,7 @@
       <c r="F48" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G48" s="26" t="s">
+      <c r="G48" s="13" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1384,7 +1391,7 @@
       <c r="F49" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G49" s="26" t="s">
+      <c r="G49" s="13" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1402,7 +1409,7 @@
       <c r="F50" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G50" s="26" t="s">
+      <c r="G50" s="13" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1420,92 +1427,92 @@
       <c r="F51" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="26" t="s">
+      <c r="G51" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D55" s="30" t="s">
+      <c r="D55" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E55" s="30" t="s">
+      <c r="E55" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F55" s="30" t="s">
+      <c r="F55" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="27" t="s">
+      <c r="B56" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C56" s="31">
+      <c r="C56" s="18">
         <v>700</v>
       </c>
-      <c r="D56" s="31">
+      <c r="D56" s="18">
         <v>720</v>
       </c>
-      <c r="E56" s="31">
+      <c r="E56" s="18">
         <v>720</v>
       </c>
-      <c r="F56" s="31">
+      <c r="F56" s="18">
         <v>720</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C57" s="31">
+      <c r="C57" s="18">
         <v>500</v>
       </c>
-      <c r="D57" s="31">
+      <c r="D57" s="18">
         <v>500</v>
       </c>
-      <c r="E57" s="31">
+      <c r="E57" s="18">
         <v>500</v>
       </c>
-      <c r="F57" s="31">
+      <c r="F57" s="18">
         <v>500</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C58" s="32">
+      <c r="C58" s="19">
         <v>600</v>
       </c>
-      <c r="D58" s="31">
+      <c r="D58" s="18">
         <v>500</v>
       </c>
-      <c r="E58" s="31">
+      <c r="E58" s="18">
         <v>500</v>
       </c>
-      <c r="F58" s="31">
+      <c r="F58" s="18">
         <v>500</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D61" s="33" t="s">
+      <c r="D61" s="20" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1525,51 +1532,51 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="12" t="s">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="27" t="s">
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="27" t="s">
+      <c r="C67" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D67" s="27" t="s">
+      <c r="D67" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E67" s="27" t="s">
+      <c r="E67" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="28" t="s">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C68" s="28" t="s">
+      <c r="C68" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D68" s="28" t="s">
+      <c r="D68" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E68" s="28" t="s">
+      <c r="E68" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="26"/>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E69" s="13"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="7"/>
       <c r="C70" s="7" t="s">
         <v>65</v>
@@ -1577,11 +1584,11 @@
       <c r="D70" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E70" s="26" t="s">
+      <c r="E70" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="7"/>
       <c r="C71" s="7" t="s">
         <v>65</v>
@@ -1589,101 +1596,229 @@
       <c r="D71" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E71" s="26" t="s">
+      <c r="E71" s="13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="7"/>
-      <c r="C72" s="34" t="s">
+      <c r="C72" s="21" t="s">
         <v>53</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E72" s="26" t="s">
+      <c r="E72" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="7"/>
-      <c r="C73" s="34" t="s">
+      <c r="C73" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D73" s="34" t="s">
+      <c r="D73" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E73" s="26" t="s">
+      <c r="E73" s="13" t="s">
         <v>69</v>
       </c>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-    </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-    </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-    </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I78" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F79" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G79" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H79" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I79" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="13"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="7"/>
+      <c r="C81" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="13">
+        <v>53650</v>
+      </c>
+      <c r="H81" s="6">
+        <v>53750</v>
+      </c>
+      <c r="I81">
+        <v>53850</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="7"/>
+      <c r="C82" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G82" s="13">
+        <v>47750</v>
+      </c>
+      <c r="H82" s="6">
+        <v>47750</v>
+      </c>
+      <c r="I82">
+        <v>47750</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="7"/>
+      <c r="C83" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G83" s="13">
+        <v>94200</v>
+      </c>
+      <c r="H83">
+        <v>95200</v>
+      </c>
+      <c r="I83">
+        <v>96200</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="7"/>
+      <c r="C84" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G84" s="13">
+        <v>91400</v>
+      </c>
+      <c r="H84">
+        <v>92400</v>
+      </c>
+      <c r="I84">
+        <v>93400</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="B77:G77"/>
     <mergeCell ref="B66:E66"/>
     <mergeCell ref="B54:F54"/>
     <mergeCell ref="B41:G41"/>

</xml_diff>